<commit_message>
ASKAPSDP-2902 adding deconvolved values for position angle, major axis, and minor axis to ICE data api
</commit_message>
<xml_diff>
--- a/Code/Components/Services/skymodel/service/schema_definitions/GSM_casda.continuum_component_description.xlsx
+++ b/Code/Components/Services/skymodel/service/schema_definitions/GSM_casda.continuum_component_description.xlsx
@@ -12,10 +12,11 @@
     <sheet name="Comparison with Selavy" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Catalogue description'!$A$1:$L$43</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Catalogue description'!$A$2:$L$37</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Catalogue description'!$A$2:$L$37</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Catalogue description'!$A$1:$L$43</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Catalogue description'!$A$2:$L$37</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Catalogue description'!$A$2:$L$37</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Catalogue description'!$A$2:$L$37</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -969,7 +970,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in TableStyleLight1" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1061,16 +1062,16 @@
   <dimension ref="A1:AMJ43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="I39" activeCellId="0" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="68.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="40.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="40.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="20.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="8.85"/>
@@ -12068,7 +12069,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" s="15" t="n">
         <v>0</v>
@@ -12104,7 +12105,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" s="15" t="n">
         <v>0</v>
@@ -12140,7 +12141,7 @@
         <v>0</v>
       </c>
       <c r="I27" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" s="15" t="n">
         <v>0</v>
@@ -12678,7 +12679,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L43"/>
+  <autoFilter ref="A2:L37"/>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
@@ -12763,7 +12764,7 @@
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="1" sqref="1:1 C15"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>